<commit_message>
clean up Napoleon u Stalder
</commit_message>
<xml_diff>
--- a/Datasets/Stalder/Data/Stalder_JR.xlsx
+++ b/Datasets/Stalder/Data/Stalder_JR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julerickert/Documents/Akademie_Projekt/Datasets/Stalder/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CD0F37E-6D08-934E-A86C-D4AF3F70EFA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C580C1FB-856E-F347-97BE-4A1872897709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{83D778BB-B2D8-FD4F-A694-2AEDDD4D8C05}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" xr2:uid="{83D778BB-B2D8-FD4F-A694-2AEDDD4D8C05}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1157" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1156" uniqueCount="458">
   <si>
     <t>ID</t>
   </si>
@@ -141,9 +141,6 @@
   </si>
   <si>
     <t>Nicht unbedingt zeitlich relevant</t>
-  </si>
-  <si>
-    <t>?</t>
   </si>
   <si>
     <t>Nicht unbedingt zeitlich relevant / Der Althochdeutsche Tatian ist eine Übersetzung der Evangelienharmonie Tatians ins Althochdeutsche. Die Übersetzung wurde um das Jahr 830 im Kloster Fulda unter der Leitung von Hrabanus Maurus angefertigt und befindet sich seit dem 10. Jahrhundert im Kloster St. Gallen (Cod. Sang. 56) {-Wikipedia}</t>
@@ -1819,7 +1816,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N111" sqref="N111"/>
+      <selection pane="bottomLeft" activeCell="Z4" sqref="Z4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1930,7 +1927,7 @@
         <v>270</v>
       </c>
       <c r="J2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K2">
         <v>999</v>
@@ -1971,22 +1968,22 @@
         <v>267</v>
       </c>
       <c r="J3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L3" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="N3" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="M3" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="N3" s="7" t="s">
+      <c r="O3" s="7" t="s">
         <v>40</v>
-      </c>
-      <c r="O3" s="7" t="s">
-        <v>41</v>
       </c>
       <c r="V3" t="s">
         <v>32</v>
@@ -1995,7 +1992,7 @@
         <v>33</v>
       </c>
       <c r="Z3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.2">
@@ -2012,31 +2009,31 @@
         <v>269</v>
       </c>
       <c r="J4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K4" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="N4" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="L4" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="M4" s="6" t="s">
+      <c r="O4" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="V4" t="s">
         <v>42</v>
-      </c>
-      <c r="N4" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="O4" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="V4" t="s">
-        <v>43</v>
       </c>
       <c r="W4" t="s">
         <v>33</v>
       </c>
       <c r="Z4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.2">
@@ -2049,29 +2046,29 @@
       <c r="D5">
         <v>271</v>
       </c>
-      <c r="E5" t="s">
-        <v>35</v>
+      <c r="E5">
+        <v>346</v>
       </c>
       <c r="J5" t="s">
+        <v>47</v>
+      </c>
+      <c r="K5" t="s">
+        <v>49</v>
+      </c>
+      <c r="L5" t="s">
+        <v>50</v>
+      </c>
+      <c r="M5" t="s">
+        <v>51</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="V5" t="s">
         <v>48</v>
-      </c>
-      <c r="K5" t="s">
-        <v>50</v>
-      </c>
-      <c r="L5" t="s">
-        <v>51</v>
-      </c>
-      <c r="M5" t="s">
-        <v>52</v>
-      </c>
-      <c r="N5" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="O5" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="V5" t="s">
-        <v>49</v>
       </c>
       <c r="W5" t="s">
         <v>31</v>
@@ -2091,25 +2088,25 @@
         <v>276</v>
       </c>
       <c r="J6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L6" t="s">
+        <v>50</v>
+      </c>
+      <c r="M6" t="s">
         <v>51</v>
       </c>
-      <c r="M6" t="s">
-        <v>52</v>
-      </c>
       <c r="N6" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O6" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="V6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="W6" t="s">
         <v>33</v>
@@ -2129,34 +2126,34 @@
         <v>274</v>
       </c>
       <c r="J7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K7" t="s">
+        <v>111</v>
+      </c>
+      <c r="L7" t="s">
+        <v>50</v>
+      </c>
+      <c r="M7" t="s">
+        <v>37</v>
+      </c>
+      <c r="N7" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="L7" t="s">
-        <v>51</v>
-      </c>
-      <c r="M7" t="s">
-        <v>38</v>
-      </c>
-      <c r="N7" s="5" t="s">
+      <c r="O7" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="O7" s="5" t="s">
-        <v>114</v>
-      </c>
       <c r="P7" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q7" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="V7" t="s">
+        <v>55</v>
+      </c>
+      <c r="W7" t="s">
         <v>56</v>
-      </c>
-      <c r="W7" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.2">
@@ -2173,28 +2170,28 @@
         <v>276</v>
       </c>
       <c r="J8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="O8" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="V8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="W8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.2">
@@ -2211,25 +2208,25 @@
         <v>289</v>
       </c>
       <c r="J9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K9" t="s">
+        <v>64</v>
+      </c>
+      <c r="L9" t="s">
+        <v>50</v>
+      </c>
+      <c r="M9" t="s">
+        <v>51</v>
+      </c>
+      <c r="N9" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="O9" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="L9" t="s">
-        <v>51</v>
-      </c>
-      <c r="M9" t="s">
-        <v>52</v>
-      </c>
-      <c r="N9" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="O9" s="5" t="s">
-        <v>66</v>
-      </c>
       <c r="V9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="W9" t="s">
         <v>33</v>
@@ -2249,28 +2246,28 @@
         <v>278</v>
       </c>
       <c r="J10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K10" t="s">
+        <v>69</v>
+      </c>
+      <c r="L10" t="s">
+        <v>38</v>
+      </c>
+      <c r="M10" t="s">
+        <v>41</v>
+      </c>
+      <c r="N10" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="L10" t="s">
-        <v>39</v>
-      </c>
-      <c r="M10" t="s">
-        <v>42</v>
-      </c>
-      <c r="N10" s="5" t="s">
+      <c r="O10" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="O10" s="5" t="s">
-        <v>72</v>
-      </c>
       <c r="V10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="W10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.2">
@@ -2287,28 +2284,28 @@
         <v>279</v>
       </c>
       <c r="J11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K11" t="s">
+        <v>73</v>
+      </c>
+      <c r="L11" t="s">
+        <v>38</v>
+      </c>
+      <c r="M11" t="s">
+        <v>37</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="O11" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="L11" t="s">
-        <v>39</v>
-      </c>
-      <c r="M11" t="s">
-        <v>38</v>
-      </c>
-      <c r="N11" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="O11" s="5" t="s">
-        <v>75</v>
-      </c>
       <c r="V11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="W11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.2">
@@ -2325,28 +2322,28 @@
         <v>289</v>
       </c>
       <c r="J12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K12" t="s">
+        <v>77</v>
+      </c>
+      <c r="L12" t="s">
+        <v>50</v>
+      </c>
+      <c r="M12" t="s">
+        <v>51</v>
+      </c>
+      <c r="N12" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="L12" t="s">
-        <v>51</v>
-      </c>
-      <c r="M12" t="s">
-        <v>52</v>
-      </c>
-      <c r="N12" s="5" t="s">
+      <c r="O12" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="O12" s="5" t="s">
-        <v>80</v>
-      </c>
       <c r="V12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="W12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.2">
@@ -2363,28 +2360,28 @@
         <v>281</v>
       </c>
       <c r="J13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N13" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="O13" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="O13" s="5" t="s">
-        <v>86</v>
-      </c>
       <c r="V13" t="s">
+        <v>80</v>
+      </c>
+      <c r="W13" t="s">
         <v>81</v>
-      </c>
-      <c r="W13" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.2">
@@ -2401,28 +2398,28 @@
         <v>283</v>
       </c>
       <c r="J14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K14" t="s">
+        <v>86</v>
+      </c>
+      <c r="L14" t="s">
+        <v>50</v>
+      </c>
+      <c r="M14" t="s">
+        <v>41</v>
+      </c>
+      <c r="N14" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="O14" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="L14" t="s">
-        <v>51</v>
-      </c>
-      <c r="M14" t="s">
-        <v>42</v>
-      </c>
-      <c r="N14" s="5" t="s">
+      <c r="V14" t="s">
         <v>89</v>
       </c>
-      <c r="O14" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="V14" t="s">
-        <v>90</v>
-      </c>
       <c r="W14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.2">
@@ -2439,28 +2436,28 @@
         <v>284</v>
       </c>
       <c r="J15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K15" t="s">
+        <v>91</v>
+      </c>
+      <c r="L15" t="s">
+        <v>50</v>
+      </c>
+      <c r="M15" t="s">
+        <v>41</v>
+      </c>
+      <c r="N15" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="O15" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="L15" t="s">
-        <v>51</v>
-      </c>
-      <c r="M15" t="s">
-        <v>42</v>
-      </c>
-      <c r="N15" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="O15" s="5" t="s">
-        <v>93</v>
-      </c>
       <c r="V15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="W15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.2">
@@ -2477,28 +2474,28 @@
         <v>286</v>
       </c>
       <c r="J16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N16" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="O16" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="V16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="W16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="2:23" x14ac:dyDescent="0.2">
@@ -2515,28 +2512,28 @@
         <v>288</v>
       </c>
       <c r="J17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K17" t="s">
+        <v>99</v>
+      </c>
+      <c r="L17" t="s">
+        <v>50</v>
+      </c>
+      <c r="M17" t="s">
+        <v>37</v>
+      </c>
+      <c r="N17" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="L17" t="s">
-        <v>51</v>
-      </c>
-      <c r="M17" t="s">
-        <v>38</v>
-      </c>
-      <c r="N17" s="5" t="s">
+      <c r="O17" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="O17" s="5" t="s">
-        <v>102</v>
-      </c>
       <c r="V17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="W17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="2:23" x14ac:dyDescent="0.2">
@@ -2553,28 +2550,28 @@
         <v>289</v>
       </c>
       <c r="J18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K18" t="s">
+        <v>103</v>
+      </c>
+      <c r="L18" t="s">
+        <v>50</v>
+      </c>
+      <c r="M18" t="s">
+        <v>41</v>
+      </c>
+      <c r="N18" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="O18" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="L18" t="s">
-        <v>51</v>
-      </c>
-      <c r="M18" t="s">
-        <v>42</v>
-      </c>
-      <c r="N18" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="O18" s="5" t="s">
-        <v>105</v>
-      </c>
       <c r="V18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="W18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="2:23" x14ac:dyDescent="0.2">
@@ -2591,25 +2588,25 @@
         <v>293</v>
       </c>
       <c r="J19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K19" t="s">
+        <v>107</v>
+      </c>
+      <c r="L19" t="s">
+        <v>50</v>
+      </c>
+      <c r="M19" t="s">
+        <v>51</v>
+      </c>
+      <c r="N19" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="L19" t="s">
-        <v>51</v>
-      </c>
-      <c r="M19" t="s">
-        <v>52</v>
-      </c>
-      <c r="N19" s="5" t="s">
+      <c r="O19" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="O19" s="5" t="s">
-        <v>110</v>
-      </c>
       <c r="V19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="W19" t="s">
         <v>33</v>
@@ -2629,28 +2626,28 @@
         <v>291</v>
       </c>
       <c r="J20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K20" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N20" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="O20" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="O20" s="5" t="s">
+      <c r="V20" t="s">
         <v>110</v>
       </c>
-      <c r="V20" t="s">
-        <v>111</v>
-      </c>
       <c r="W20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="2:23" x14ac:dyDescent="0.2">
@@ -2667,28 +2664,28 @@
         <v>293</v>
       </c>
       <c r="J21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K21" t="s">
+        <v>116</v>
+      </c>
+      <c r="L21" t="s">
+        <v>50</v>
+      </c>
+      <c r="M21" t="s">
+        <v>41</v>
+      </c>
+      <c r="N21" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="L21" t="s">
-        <v>51</v>
-      </c>
-      <c r="M21" t="s">
-        <v>42</v>
-      </c>
-      <c r="N21" s="5" t="s">
+      <c r="O21" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="O21" s="5" t="s">
-        <v>119</v>
-      </c>
       <c r="V21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="W21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="2:23" x14ac:dyDescent="0.2">
@@ -2705,25 +2702,25 @@
         <v>294</v>
       </c>
       <c r="J22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K22" t="s">
+        <v>120</v>
+      </c>
+      <c r="L22" t="s">
+        <v>50</v>
+      </c>
+      <c r="M22" t="s">
+        <v>37</v>
+      </c>
+      <c r="N22" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="O22" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="L22" t="s">
-        <v>51</v>
-      </c>
-      <c r="M22" t="s">
-        <v>38</v>
-      </c>
-      <c r="N22" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="O22" s="5" t="s">
-        <v>122</v>
-      </c>
       <c r="V22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="W22" t="s">
         <v>33</v>
@@ -2743,28 +2740,28 @@
         <v>294</v>
       </c>
       <c r="J23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K23" t="s">
+        <v>124</v>
+      </c>
+      <c r="L23" t="s">
+        <v>50</v>
+      </c>
+      <c r="M23" t="s">
+        <v>37</v>
+      </c>
+      <c r="N23" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="L23" t="s">
-        <v>51</v>
-      </c>
-      <c r="M23" t="s">
-        <v>38</v>
-      </c>
-      <c r="N23" s="5" t="s">
+      <c r="O23" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="O23" s="5" t="s">
-        <v>127</v>
-      </c>
       <c r="V23" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="W23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="2:23" x14ac:dyDescent="0.2">
@@ -2781,25 +2778,25 @@
         <v>296</v>
       </c>
       <c r="J24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K24" t="s">
+        <v>128</v>
+      </c>
+      <c r="L24" t="s">
+        <v>50</v>
+      </c>
+      <c r="M24" t="s">
+        <v>37</v>
+      </c>
+      <c r="N24" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="L24" t="s">
-        <v>51</v>
-      </c>
-      <c r="M24" t="s">
-        <v>38</v>
-      </c>
-      <c r="N24" s="5" t="s">
+      <c r="O24" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="O24" s="5" t="s">
-        <v>131</v>
-      </c>
       <c r="V24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="W24" t="s">
         <v>33</v>
@@ -2819,28 +2816,28 @@
         <v>296</v>
       </c>
       <c r="J25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K25" t="s">
+        <v>132</v>
+      </c>
+      <c r="L25" t="s">
+        <v>50</v>
+      </c>
+      <c r="M25" t="s">
+        <v>41</v>
+      </c>
+      <c r="N25" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="O25" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="L25" t="s">
-        <v>51</v>
-      </c>
-      <c r="M25" t="s">
-        <v>42</v>
-      </c>
-      <c r="N25" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="O25" s="5" t="s">
-        <v>134</v>
-      </c>
       <c r="V25" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="W25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="2:23" x14ac:dyDescent="0.2">
@@ -2857,25 +2854,25 @@
         <v>300</v>
       </c>
       <c r="J26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K26" t="s">
+        <v>135</v>
+      </c>
+      <c r="L26" t="s">
+        <v>50</v>
+      </c>
+      <c r="M26" t="s">
+        <v>37</v>
+      </c>
+      <c r="N26" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="L26" t="s">
-        <v>51</v>
-      </c>
-      <c r="M26" t="s">
-        <v>38</v>
-      </c>
-      <c r="N26" s="5" t="s">
+      <c r="O26" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="O26" s="5" t="s">
-        <v>138</v>
-      </c>
       <c r="V26" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="W26" t="s">
         <v>33</v>
@@ -2895,28 +2892,28 @@
         <v>298</v>
       </c>
       <c r="J27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K27" t="s">
+        <v>138</v>
+      </c>
+      <c r="L27" t="s">
+        <v>50</v>
+      </c>
+      <c r="M27" t="s">
+        <v>37</v>
+      </c>
+      <c r="N27" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="O27" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="L27" t="s">
-        <v>51</v>
-      </c>
-      <c r="M27" t="s">
-        <v>38</v>
-      </c>
-      <c r="N27" s="5" t="s">
+      <c r="V27" t="s">
         <v>141</v>
       </c>
-      <c r="O27" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="V27" t="s">
-        <v>142</v>
-      </c>
       <c r="W27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="2:23" x14ac:dyDescent="0.2">
@@ -2933,28 +2930,28 @@
         <v>300</v>
       </c>
       <c r="J28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K28" t="s">
+        <v>143</v>
+      </c>
+      <c r="L28" t="s">
+        <v>50</v>
+      </c>
+      <c r="M28" t="s">
+        <v>37</v>
+      </c>
+      <c r="N28" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="O28" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="L28" t="s">
-        <v>51</v>
-      </c>
-      <c r="M28" t="s">
-        <v>38</v>
-      </c>
-      <c r="N28" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="O28" s="5" t="s">
-        <v>145</v>
-      </c>
       <c r="V28" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="W28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="2:23" x14ac:dyDescent="0.2">
@@ -2971,25 +2968,25 @@
         <v>302</v>
       </c>
       <c r="J29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K29" t="s">
+        <v>147</v>
+      </c>
+      <c r="L29" t="s">
+        <v>50</v>
+      </c>
+      <c r="M29" t="s">
+        <v>37</v>
+      </c>
+      <c r="N29" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="L29" t="s">
-        <v>51</v>
-      </c>
-      <c r="M29" t="s">
-        <v>38</v>
-      </c>
-      <c r="N29" s="5" t="s">
+      <c r="O29" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="O29" s="5" t="s">
-        <v>150</v>
-      </c>
       <c r="V29" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="W29" t="s">
         <v>33</v>
@@ -3009,34 +3006,34 @@
         <v>302</v>
       </c>
       <c r="J30" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K30" t="s">
+        <v>151</v>
+      </c>
+      <c r="L30" t="s">
+        <v>50</v>
+      </c>
+      <c r="M30" t="s">
+        <v>37</v>
+      </c>
+      <c r="N30" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="O30" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="L30" t="s">
-        <v>51</v>
-      </c>
-      <c r="M30" t="s">
-        <v>38</v>
-      </c>
-      <c r="N30" s="5" t="s">
+      <c r="P30" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q30" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="O30" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="P30" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="Q30" s="5" t="s">
-        <v>155</v>
-      </c>
       <c r="V30" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="W30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="2:23" x14ac:dyDescent="0.2">
@@ -3053,25 +3050,25 @@
         <v>304</v>
       </c>
       <c r="J31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K31" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L31" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N31" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="O31" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="O31" s="5" t="s">
-        <v>159</v>
-      </c>
       <c r="V31" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="W31" t="s">
         <v>33</v>
@@ -3091,28 +3088,28 @@
         <v>304</v>
       </c>
       <c r="J32" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M32" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N32" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="O32" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="O32" s="5" t="s">
+      <c r="V32" t="s">
         <v>159</v>
       </c>
-      <c r="V32" t="s">
-        <v>160</v>
-      </c>
       <c r="W32" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="2:26" x14ac:dyDescent="0.2">
@@ -3129,25 +3126,25 @@
         <v>307</v>
       </c>
       <c r="J33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K33" t="s">
+        <v>163</v>
+      </c>
+      <c r="L33" t="s">
+        <v>50</v>
+      </c>
+      <c r="M33" t="s">
+        <v>37</v>
+      </c>
+      <c r="N33" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="O33" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="L33" t="s">
-        <v>51</v>
-      </c>
-      <c r="M33" t="s">
-        <v>38</v>
-      </c>
-      <c r="N33" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="O33" s="5" t="s">
-        <v>165</v>
-      </c>
       <c r="V33" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="W33" t="s">
         <v>33</v>
@@ -3167,28 +3164,28 @@
         <v>305</v>
       </c>
       <c r="J34" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K34" t="s">
+        <v>167</v>
+      </c>
+      <c r="L34" t="s">
+        <v>50</v>
+      </c>
+      <c r="M34" t="s">
+        <v>37</v>
+      </c>
+      <c r="N34" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="L34" t="s">
-        <v>51</v>
-      </c>
-      <c r="M34" t="s">
-        <v>38</v>
-      </c>
-      <c r="N34" s="5" t="s">
+      <c r="O34" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="O34" s="5" t="s">
-        <v>170</v>
-      </c>
       <c r="V34" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="W34" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="2:26" x14ac:dyDescent="0.2">
@@ -3205,28 +3202,28 @@
         <v>307</v>
       </c>
       <c r="J35" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K35" t="s">
+        <v>171</v>
+      </c>
+      <c r="L35" t="s">
+        <v>50</v>
+      </c>
+      <c r="M35" t="s">
+        <v>37</v>
+      </c>
+      <c r="N35" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="L35" t="s">
-        <v>51</v>
-      </c>
-      <c r="M35" t="s">
-        <v>38</v>
-      </c>
-      <c r="N35" s="5" t="s">
+      <c r="O35" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="O35" s="5" t="s">
-        <v>174</v>
-      </c>
       <c r="V35" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="W35" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="36" spans="2:26" x14ac:dyDescent="0.2">
@@ -3243,25 +3240,25 @@
         <v>309</v>
       </c>
       <c r="J36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K36" t="s">
+        <v>174</v>
+      </c>
+      <c r="L36" t="s">
+        <v>50</v>
+      </c>
+      <c r="M36" t="s">
+        <v>51</v>
+      </c>
+      <c r="N36" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="O36" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="V36" t="s">
         <v>175</v>
-      </c>
-      <c r="L36" t="s">
-        <v>51</v>
-      </c>
-      <c r="M36" t="s">
-        <v>52</v>
-      </c>
-      <c r="N36" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="O36" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="V36" t="s">
-        <v>176</v>
       </c>
       <c r="W36" t="s">
         <v>33</v>
@@ -3281,28 +3278,28 @@
         <v>309</v>
       </c>
       <c r="J37" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K37" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="L37" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M37" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N37" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="O37" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="O37" s="5" t="s">
+      <c r="V37" t="s">
         <v>178</v>
       </c>
-      <c r="V37" t="s">
-        <v>179</v>
-      </c>
       <c r="W37" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="38" spans="2:26" x14ac:dyDescent="0.2">
@@ -3319,25 +3316,25 @@
         <v>310</v>
       </c>
       <c r="J38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K38" t="s">
+        <v>181</v>
+      </c>
+      <c r="L38" t="s">
+        <v>50</v>
+      </c>
+      <c r="M38" t="s">
+        <v>37</v>
+      </c>
+      <c r="N38" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="L38" t="s">
-        <v>51</v>
-      </c>
-      <c r="M38" t="s">
-        <v>38</v>
-      </c>
-      <c r="N38" s="5" t="s">
+      <c r="O38" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="O38" s="5" t="s">
-        <v>184</v>
-      </c>
       <c r="V38" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="W38" t="s">
         <v>33</v>
@@ -3357,28 +3354,28 @@
         <v>310</v>
       </c>
       <c r="J39" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K39" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="L39" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N39" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="O39" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="O39" s="5" t="s">
+      <c r="V39" t="s">
         <v>184</v>
       </c>
-      <c r="V39" t="s">
-        <v>185</v>
-      </c>
       <c r="W39" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="40" spans="2:26" x14ac:dyDescent="0.2">
@@ -3395,31 +3392,31 @@
         <v>312</v>
       </c>
       <c r="J40" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K40" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="L40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N40" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="O40" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="V40" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="W40" t="s">
         <v>33</v>
       </c>
       <c r="Z40" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="41" spans="2:26" x14ac:dyDescent="0.2">
@@ -3436,31 +3433,31 @@
         <v>312</v>
       </c>
       <c r="J41" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K41" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="L41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N41" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="O41" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="V41" t="s">
+        <v>187</v>
+      </c>
+      <c r="W41" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z41" t="s">
         <v>194</v>
-      </c>
-      <c r="O41" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="V41" t="s">
-        <v>188</v>
-      </c>
-      <c r="W41" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z41" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="42" spans="2:26" x14ac:dyDescent="0.2">
@@ -3477,25 +3474,25 @@
         <v>314</v>
       </c>
       <c r="J42" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K42" t="s">
+        <v>197</v>
+      </c>
+      <c r="L42" t="s">
+        <v>50</v>
+      </c>
+      <c r="M42" t="s">
+        <v>37</v>
+      </c>
+      <c r="N42" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="L42" t="s">
-        <v>51</v>
-      </c>
-      <c r="M42" t="s">
-        <v>38</v>
-      </c>
-      <c r="N42" s="5" t="s">
+      <c r="O42" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="O42" s="5" t="s">
-        <v>200</v>
-      </c>
       <c r="V42" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="W42" t="s">
         <v>33</v>
@@ -3515,28 +3512,28 @@
         <v>314</v>
       </c>
       <c r="J43" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K43" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L43" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M43" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N43" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="O43" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="O43" s="5" t="s">
-        <v>200</v>
-      </c>
       <c r="V43" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="W43" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="44" spans="2:26" x14ac:dyDescent="0.2">
@@ -3553,25 +3550,25 @@
         <v>323</v>
       </c>
       <c r="J44" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K44" t="s">
+        <v>202</v>
+      </c>
+      <c r="L44" t="s">
+        <v>50</v>
+      </c>
+      <c r="M44" t="s">
+        <v>51</v>
+      </c>
+      <c r="N44" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="O44" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="L44" t="s">
-        <v>51</v>
-      </c>
-      <c r="M44" t="s">
-        <v>52</v>
-      </c>
-      <c r="N44" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="O44" s="5" t="s">
-        <v>204</v>
-      </c>
       <c r="V44" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="W44" t="s">
         <v>33</v>
@@ -3591,34 +3588,34 @@
         <v>316</v>
       </c>
       <c r="J45" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K45" t="s">
+        <v>206</v>
+      </c>
+      <c r="L45" t="s">
+        <v>38</v>
+      </c>
+      <c r="M45" t="s">
+        <v>37</v>
+      </c>
+      <c r="N45" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="O45" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="P45" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="Q45" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="L45" t="s">
-        <v>39</v>
-      </c>
-      <c r="M45" t="s">
-        <v>38</v>
-      </c>
-      <c r="N45" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="O45" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="P45" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="Q45" s="5" t="s">
-        <v>208</v>
-      </c>
       <c r="V45" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="W45" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="46" spans="2:26" x14ac:dyDescent="0.2">
@@ -3635,28 +3632,28 @@
         <v>323</v>
       </c>
       <c r="J46" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K46" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L46" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M46" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N46" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="O46" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="O46" s="5" t="s">
-        <v>215</v>
-      </c>
       <c r="V46" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="W46" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="47" spans="2:26" x14ac:dyDescent="0.2">
@@ -3673,28 +3670,28 @@
         <v>317</v>
       </c>
       <c r="J47" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K47" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="L47" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M47" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N47" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="O47" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="V47" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="W47" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="48" spans="2:26" x14ac:dyDescent="0.2">
@@ -3711,28 +3708,28 @@
         <v>319</v>
       </c>
       <c r="J48" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K48" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="L48" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M48" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N48" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="O48" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="V48" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="W48" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="49" spans="2:23" x14ac:dyDescent="0.2">
@@ -3749,28 +3746,28 @@
         <v>321</v>
       </c>
       <c r="J49" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K49" t="s">
+        <v>221</v>
+      </c>
+      <c r="L49" t="s">
+        <v>50</v>
+      </c>
+      <c r="M49" t="s">
+        <v>37</v>
+      </c>
+      <c r="N49" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="O49" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="L49" t="s">
-        <v>51</v>
-      </c>
-      <c r="M49" t="s">
-        <v>38</v>
-      </c>
-      <c r="N49" s="5" t="s">
+      <c r="V49" t="s">
         <v>224</v>
       </c>
-      <c r="O49" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="V49" t="s">
-        <v>225</v>
-      </c>
       <c r="W49" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="50" spans="2:23" x14ac:dyDescent="0.2">
@@ -3787,28 +3784,28 @@
         <v>323</v>
       </c>
       <c r="J50" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K50" t="s">
+        <v>226</v>
+      </c>
+      <c r="L50" t="s">
+        <v>50</v>
+      </c>
+      <c r="M50" t="s">
+        <v>37</v>
+      </c>
+      <c r="N50" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="O50" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="L50" t="s">
-        <v>51</v>
-      </c>
-      <c r="M50" t="s">
-        <v>38</v>
-      </c>
-      <c r="N50" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="O50" s="5" t="s">
-        <v>228</v>
-      </c>
       <c r="V50" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="W50" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="51" spans="2:23" x14ac:dyDescent="0.2">
@@ -3825,25 +3822,25 @@
         <v>328</v>
       </c>
       <c r="J51" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K51" t="s">
+        <v>230</v>
+      </c>
+      <c r="L51" t="s">
+        <v>50</v>
+      </c>
+      <c r="M51" t="s">
+        <v>51</v>
+      </c>
+      <c r="N51" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="O51" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="L51" t="s">
-        <v>51</v>
-      </c>
-      <c r="M51" t="s">
-        <v>52</v>
-      </c>
-      <c r="N51" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="O51" s="5" t="s">
-        <v>232</v>
-      </c>
       <c r="V51" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="W51" t="s">
         <v>33</v>
@@ -3863,28 +3860,28 @@
         <v>324</v>
       </c>
       <c r="J52" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K52" t="s">
+        <v>234</v>
+      </c>
+      <c r="L52" t="s">
+        <v>50</v>
+      </c>
+      <c r="M52" t="s">
+        <v>37</v>
+      </c>
+      <c r="N52" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="L52" t="s">
-        <v>51</v>
-      </c>
-      <c r="M52" t="s">
-        <v>38</v>
-      </c>
-      <c r="N52" s="5" t="s">
+      <c r="O52" s="5" t="s">
         <v>236</v>
       </c>
-      <c r="O52" s="5" t="s">
-        <v>237</v>
-      </c>
       <c r="V52" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="W52" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="53" spans="2:23" x14ac:dyDescent="0.2">
@@ -3901,28 +3898,28 @@
         <v>326</v>
       </c>
       <c r="J53" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K53" t="s">
+        <v>237</v>
+      </c>
+      <c r="L53" t="s">
+        <v>50</v>
+      </c>
+      <c r="M53" t="s">
+        <v>37</v>
+      </c>
+      <c r="N53" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="O53" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="V53" t="s">
         <v>238</v>
       </c>
-      <c r="L53" t="s">
-        <v>51</v>
-      </c>
-      <c r="M53" t="s">
-        <v>38</v>
-      </c>
-      <c r="N53" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="O53" s="5" t="s">
-        <v>240</v>
-      </c>
-      <c r="V53" t="s">
-        <v>239</v>
-      </c>
       <c r="W53" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="54" spans="2:23" x14ac:dyDescent="0.2">
@@ -3939,28 +3936,28 @@
         <v>328</v>
       </c>
       <c r="J54" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K54" t="s">
+        <v>242</v>
+      </c>
+      <c r="L54" t="s">
+        <v>50</v>
+      </c>
+      <c r="M54" t="s">
+        <v>37</v>
+      </c>
+      <c r="N54" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="O54" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="L54" t="s">
-        <v>51</v>
-      </c>
-      <c r="M54" t="s">
-        <v>38</v>
-      </c>
-      <c r="N54" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="O54" s="5" t="s">
-        <v>244</v>
-      </c>
       <c r="V54" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="W54" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="55" spans="2:23" x14ac:dyDescent="0.2">
@@ -3977,25 +3974,25 @@
         <v>335</v>
       </c>
       <c r="J55" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K55" t="s">
+        <v>246</v>
+      </c>
+      <c r="L55" t="s">
+        <v>50</v>
+      </c>
+      <c r="M55" t="s">
+        <v>37</v>
+      </c>
+      <c r="N55" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="O55" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="L55" t="s">
-        <v>51</v>
-      </c>
-      <c r="M55" t="s">
-        <v>38</v>
-      </c>
-      <c r="N55" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="O55" s="5" t="s">
-        <v>248</v>
-      </c>
       <c r="V55" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="W55" t="s">
         <v>33</v>
@@ -4015,28 +4012,28 @@
         <v>331</v>
       </c>
       <c r="J56" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K56" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="L56" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M56" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N56" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="O56" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="V56" t="s">
         <v>249</v>
       </c>
-      <c r="O56" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="V56" t="s">
-        <v>250</v>
-      </c>
       <c r="W56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="57" spans="2:23" x14ac:dyDescent="0.2">
@@ -4053,34 +4050,34 @@
         <v>329</v>
       </c>
       <c r="J57" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K57" t="s">
+        <v>252</v>
+      </c>
+      <c r="L57" t="s">
+        <v>50</v>
+      </c>
+      <c r="M57" t="s">
+        <v>37</v>
+      </c>
+      <c r="N57" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="O57" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="P57" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="Q57" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="L57" t="s">
-        <v>51</v>
-      </c>
-      <c r="M57" t="s">
-        <v>38</v>
-      </c>
-      <c r="N57" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="O57" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="P57" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="Q57" s="5" t="s">
-        <v>254</v>
-      </c>
       <c r="V57" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="W57" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="58" spans="2:23" x14ac:dyDescent="0.2">
@@ -4097,28 +4094,28 @@
         <v>331</v>
       </c>
       <c r="J58" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K58" t="s">
+        <v>258</v>
+      </c>
+      <c r="L58" t="s">
+        <v>50</v>
+      </c>
+      <c r="M58" t="s">
+        <v>37</v>
+      </c>
+      <c r="N58" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="O58" s="5" t="s">
         <v>259</v>
       </c>
-      <c r="L58" t="s">
-        <v>51</v>
-      </c>
-      <c r="M58" t="s">
-        <v>38</v>
-      </c>
-      <c r="N58" s="5" t="s">
-        <v>261</v>
-      </c>
-      <c r="O58" s="5" t="s">
-        <v>260</v>
-      </c>
       <c r="V58" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="W58" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="59" spans="2:23" x14ac:dyDescent="0.2">
@@ -4135,28 +4132,28 @@
         <v>333</v>
       </c>
       <c r="J59" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K59" t="s">
+        <v>262</v>
+      </c>
+      <c r="L59" t="s">
+        <v>50</v>
+      </c>
+      <c r="M59" t="s">
+        <v>37</v>
+      </c>
+      <c r="N59" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="O59" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="L59" t="s">
-        <v>51</v>
-      </c>
-      <c r="M59" t="s">
-        <v>38</v>
-      </c>
-      <c r="N59" s="5" t="s">
-        <v>265</v>
-      </c>
-      <c r="O59" s="5" t="s">
-        <v>264</v>
-      </c>
       <c r="V59" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="W59" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="60" spans="2:23" x14ac:dyDescent="0.2">
@@ -4173,28 +4170,28 @@
         <v>335</v>
       </c>
       <c r="J60" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K60" t="s">
+        <v>266</v>
+      </c>
+      <c r="L60" t="s">
+        <v>50</v>
+      </c>
+      <c r="M60" t="s">
+        <v>37</v>
+      </c>
+      <c r="N60" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="O60" s="5" t="s">
         <v>267</v>
       </c>
-      <c r="L60" t="s">
-        <v>51</v>
-      </c>
-      <c r="M60" t="s">
-        <v>38</v>
-      </c>
-      <c r="N60" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="O60" s="5" t="s">
-        <v>268</v>
-      </c>
       <c r="V60" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="W60" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="61" spans="2:23" x14ac:dyDescent="0.2">
@@ -4211,25 +4208,25 @@
         <v>339</v>
       </c>
       <c r="J61" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K61" t="s">
+        <v>270</v>
+      </c>
+      <c r="L61" t="s">
+        <v>50</v>
+      </c>
+      <c r="M61" t="s">
+        <v>37</v>
+      </c>
+      <c r="N61" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="O61" s="5" t="s">
         <v>271</v>
       </c>
-      <c r="L61" t="s">
-        <v>51</v>
-      </c>
-      <c r="M61" t="s">
-        <v>38</v>
-      </c>
-      <c r="N61" s="5" t="s">
-        <v>273</v>
-      </c>
-      <c r="O61" s="5" t="s">
-        <v>272</v>
-      </c>
       <c r="V61" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="W61" t="s">
         <v>33</v>
@@ -4249,28 +4246,28 @@
         <v>337</v>
       </c>
       <c r="J62" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K62" t="s">
+        <v>274</v>
+      </c>
+      <c r="L62" t="s">
+        <v>50</v>
+      </c>
+      <c r="M62" t="s">
+        <v>37</v>
+      </c>
+      <c r="N62" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="L62" t="s">
-        <v>51</v>
-      </c>
-      <c r="M62" t="s">
-        <v>38</v>
-      </c>
-      <c r="N62" s="5" t="s">
+      <c r="O62" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="O62" s="5" t="s">
-        <v>277</v>
-      </c>
       <c r="V62" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="W62" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="63" spans="2:23" x14ac:dyDescent="0.2">
@@ -4287,34 +4284,34 @@
         <v>339</v>
       </c>
       <c r="J63" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K63" t="s">
+        <v>278</v>
+      </c>
+      <c r="L63" t="s">
+        <v>50</v>
+      </c>
+      <c r="M63" t="s">
+        <v>37</v>
+      </c>
+      <c r="N63" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="O63" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="L63" t="s">
-        <v>51</v>
-      </c>
-      <c r="M63" t="s">
-        <v>38</v>
-      </c>
-      <c r="N63" s="5" t="s">
+      <c r="P63" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="Q63" s="5" t="s">
         <v>281</v>
       </c>
-      <c r="O63" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="P63" s="5" t="s">
-        <v>283</v>
-      </c>
-      <c r="Q63" s="5" t="s">
-        <v>282</v>
-      </c>
       <c r="V63" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="W63" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="64" spans="2:23" x14ac:dyDescent="0.2">
@@ -4331,25 +4328,25 @@
         <v>346</v>
       </c>
       <c r="J64" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K64" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="L64" t="s">
+        <v>50</v>
+      </c>
+      <c r="M64" t="s">
         <v>51</v>
       </c>
-      <c r="M64" t="s">
-        <v>52</v>
-      </c>
       <c r="N64" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="O64" s="5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="V64" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="W64" t="s">
         <v>33</v>
@@ -4369,28 +4366,28 @@
         <v>340</v>
       </c>
       <c r="J65" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K65" t="s">
+        <v>286</v>
+      </c>
+      <c r="L65" t="s">
+        <v>50</v>
+      </c>
+      <c r="M65" t="s">
+        <v>37</v>
+      </c>
+      <c r="N65" s="5" t="s">
         <v>287</v>
       </c>
-      <c r="L65" t="s">
-        <v>51</v>
-      </c>
-      <c r="M65" t="s">
-        <v>38</v>
-      </c>
-      <c r="N65" s="5" t="s">
+      <c r="O65" s="5" t="s">
         <v>288</v>
       </c>
-      <c r="O65" s="5" t="s">
-        <v>289</v>
-      </c>
       <c r="V65" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="W65" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="66" spans="2:26" x14ac:dyDescent="0.2">
@@ -4407,34 +4404,34 @@
         <v>342</v>
       </c>
       <c r="J66" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K66" t="s">
+        <v>292</v>
+      </c>
+      <c r="L66" t="s">
+        <v>50</v>
+      </c>
+      <c r="M66" t="s">
+        <v>37</v>
+      </c>
+      <c r="N66" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="L66" t="s">
-        <v>51</v>
-      </c>
-      <c r="M66" t="s">
-        <v>38</v>
-      </c>
-      <c r="N66" s="5" t="s">
+      <c r="O66" s="5" t="s">
         <v>294</v>
       </c>
-      <c r="O66" s="5" t="s">
+      <c r="P66" s="5" t="s">
         <v>295</v>
       </c>
-      <c r="P66" s="5" t="s">
+      <c r="Q66" s="5" t="s">
         <v>296</v>
       </c>
-      <c r="Q66" s="5" t="s">
-        <v>297</v>
-      </c>
       <c r="V66" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="W66" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="67" spans="2:26" x14ac:dyDescent="0.2">
@@ -4451,28 +4448,28 @@
         <v>344</v>
       </c>
       <c r="J67" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K67" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="L67" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M67" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N67" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="O67" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="V67" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="W67" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="68" spans="2:26" x14ac:dyDescent="0.2">
@@ -4489,28 +4486,28 @@
         <v>346</v>
       </c>
       <c r="J68" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K68" t="s">
+        <v>302</v>
+      </c>
+      <c r="L68" t="s">
+        <v>50</v>
+      </c>
+      <c r="M68" t="s">
+        <v>37</v>
+      </c>
+      <c r="N68" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="O68" s="5" t="s">
         <v>303</v>
       </c>
-      <c r="L68" t="s">
-        <v>51</v>
-      </c>
-      <c r="M68" t="s">
-        <v>38</v>
-      </c>
-      <c r="N68" s="5" t="s">
-        <v>305</v>
-      </c>
-      <c r="O68" s="5" t="s">
-        <v>304</v>
-      </c>
       <c r="V68" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="W68" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="69" spans="2:26" x14ac:dyDescent="0.2">
@@ -4527,7 +4524,7 @@
         <v>360</v>
       </c>
       <c r="J69" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K69">
         <v>999</v>
@@ -4539,13 +4536,13 @@
         <v>999</v>
       </c>
       <c r="N69" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="O69" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="V69" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="W69" t="s">
         <v>31</v>
@@ -4565,25 +4562,25 @@
         <v>360</v>
       </c>
       <c r="J70" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K70" t="s">
+        <v>230</v>
+      </c>
+      <c r="L70" t="s">
+        <v>50</v>
+      </c>
+      <c r="M70" t="s">
+        <v>51</v>
+      </c>
+      <c r="N70" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="O70" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="L70" t="s">
-        <v>51</v>
-      </c>
-      <c r="M70" t="s">
-        <v>52</v>
-      </c>
-      <c r="N70" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="O70" s="5" t="s">
-        <v>232</v>
-      </c>
       <c r="V70" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="W70" t="s">
         <v>33</v>
@@ -4603,28 +4600,28 @@
         <v>353</v>
       </c>
       <c r="J71" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K71" t="s">
+        <v>77</v>
+      </c>
+      <c r="L71" t="s">
+        <v>50</v>
+      </c>
+      <c r="M71" t="s">
+        <v>51</v>
+      </c>
+      <c r="N71" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="L71" t="s">
-        <v>51</v>
-      </c>
-      <c r="M71" t="s">
-        <v>52</v>
-      </c>
-      <c r="N71" s="5" t="s">
+      <c r="O71" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="O71" s="5" t="s">
-        <v>80</v>
-      </c>
       <c r="V71" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="W71" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="72" spans="2:26" x14ac:dyDescent="0.2">
@@ -4641,31 +4638,31 @@
         <v>351</v>
       </c>
       <c r="J72" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K72" t="s">
+        <v>77</v>
+      </c>
+      <c r="L72" t="s">
+        <v>50</v>
+      </c>
+      <c r="M72" t="s">
+        <v>51</v>
+      </c>
+      <c r="N72" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="L72" t="s">
-        <v>51</v>
-      </c>
-      <c r="M72" t="s">
-        <v>52</v>
-      </c>
-      <c r="N72" s="5" t="s">
+      <c r="O72" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="O72" s="5" t="s">
-        <v>80</v>
-      </c>
       <c r="V72" t="s">
+        <v>308</v>
+      </c>
+      <c r="W72" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z72" t="s">
         <v>309</v>
-      </c>
-      <c r="W72" t="s">
-        <v>82</v>
-      </c>
-      <c r="Z72" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="73" spans="2:26" x14ac:dyDescent="0.2">
@@ -4682,28 +4679,28 @@
         <v>353</v>
       </c>
       <c r="J73" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K73" t="s">
+        <v>77</v>
+      </c>
+      <c r="L73" t="s">
+        <v>50</v>
+      </c>
+      <c r="M73" t="s">
+        <v>51</v>
+      </c>
+      <c r="N73" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="L73" t="s">
-        <v>51</v>
-      </c>
-      <c r="M73" t="s">
-        <v>52</v>
-      </c>
-      <c r="N73" s="5" t="s">
+      <c r="O73" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="O73" s="5" t="s">
-        <v>80</v>
-      </c>
       <c r="V73" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="W73" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="74" spans="2:26" x14ac:dyDescent="0.2">
@@ -4720,28 +4717,28 @@
         <v>354</v>
       </c>
       <c r="J74" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K74" t="s">
+        <v>312</v>
+      </c>
+      <c r="L74" t="s">
+        <v>50</v>
+      </c>
+      <c r="M74" t="s">
+        <v>41</v>
+      </c>
+      <c r="N74" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="O74" s="5" t="s">
         <v>313</v>
       </c>
-      <c r="L74" t="s">
-        <v>51</v>
-      </c>
-      <c r="M74" t="s">
-        <v>42</v>
-      </c>
-      <c r="N74" s="5" t="s">
-        <v>315</v>
-      </c>
-      <c r="O74" s="5" t="s">
-        <v>314</v>
-      </c>
       <c r="V74" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="W74" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="75" spans="2:26" x14ac:dyDescent="0.2">
@@ -4758,28 +4755,28 @@
         <v>355</v>
       </c>
       <c r="J75" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K75" t="s">
+        <v>316</v>
+      </c>
+      <c r="L75" t="s">
+        <v>50</v>
+      </c>
+      <c r="M75" t="s">
+        <v>37</v>
+      </c>
+      <c r="N75" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="O75" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="L75" t="s">
-        <v>51</v>
-      </c>
-      <c r="M75" t="s">
-        <v>38</v>
-      </c>
-      <c r="N75" s="5" t="s">
-        <v>319</v>
-      </c>
-      <c r="O75" s="5" t="s">
-        <v>318</v>
-      </c>
       <c r="V75" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="W75" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="76" spans="2:26" x14ac:dyDescent="0.2">
@@ -4796,28 +4793,28 @@
         <v>360</v>
       </c>
       <c r="J76" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K76" t="s">
+        <v>321</v>
+      </c>
+      <c r="L76" t="s">
+        <v>50</v>
+      </c>
+      <c r="M76" t="s">
+        <v>51</v>
+      </c>
+      <c r="N76" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="O76" s="5" t="s">
         <v>322</v>
       </c>
-      <c r="L76" t="s">
-        <v>51</v>
-      </c>
-      <c r="M76" t="s">
-        <v>52</v>
-      </c>
-      <c r="N76" s="5" t="s">
-        <v>324</v>
-      </c>
-      <c r="O76" s="5" t="s">
-        <v>323</v>
-      </c>
       <c r="V76" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="W76" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="77" spans="2:26" x14ac:dyDescent="0.2">
@@ -4834,28 +4831,28 @@
         <v>357</v>
       </c>
       <c r="J77" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K77" t="s">
+        <v>324</v>
+      </c>
+      <c r="L77" t="s">
+        <v>50</v>
+      </c>
+      <c r="M77" t="s">
+        <v>37</v>
+      </c>
+      <c r="N77" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="O77" s="5" t="s">
         <v>325</v>
       </c>
-      <c r="L77" t="s">
-        <v>51</v>
-      </c>
-      <c r="M77" t="s">
-        <v>38</v>
-      </c>
-      <c r="N77" s="5" t="s">
-        <v>327</v>
-      </c>
-      <c r="O77" s="5" t="s">
-        <v>326</v>
-      </c>
       <c r="V77" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="W77" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="78" spans="2:26" x14ac:dyDescent="0.2">
@@ -4872,28 +4869,28 @@
         <v>360</v>
       </c>
       <c r="J78" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K78" t="s">
+        <v>328</v>
+      </c>
+      <c r="L78" t="s">
+        <v>50</v>
+      </c>
+      <c r="M78" t="s">
+        <v>37</v>
+      </c>
+      <c r="N78" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="O78" s="5" t="s">
         <v>329</v>
       </c>
-      <c r="L78" t="s">
-        <v>51</v>
-      </c>
-      <c r="M78" t="s">
-        <v>38</v>
-      </c>
-      <c r="N78" s="5" t="s">
-        <v>331</v>
-      </c>
-      <c r="O78" s="5" t="s">
-        <v>330</v>
-      </c>
       <c r="V78" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="W78" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="79" spans="2:26" x14ac:dyDescent="0.2">
@@ -4910,25 +4907,25 @@
         <v>404</v>
       </c>
       <c r="J79" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K79" t="s">
+        <v>332</v>
+      </c>
+      <c r="L79" t="s">
+        <v>50</v>
+      </c>
+      <c r="M79" t="s">
+        <v>51</v>
+      </c>
+      <c r="N79" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="O79" s="5" t="s">
         <v>333</v>
       </c>
-      <c r="L79" t="s">
-        <v>51</v>
-      </c>
-      <c r="M79" t="s">
-        <v>52</v>
-      </c>
-      <c r="N79" s="5" t="s">
-        <v>335</v>
-      </c>
-      <c r="O79" s="5" t="s">
-        <v>334</v>
-      </c>
       <c r="V79" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="W79" t="s">
         <v>31</v>
@@ -4948,25 +4945,25 @@
         <v>374</v>
       </c>
       <c r="J80" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K80" t="s">
+        <v>64</v>
+      </c>
+      <c r="L80" t="s">
+        <v>50</v>
+      </c>
+      <c r="M80" t="s">
+        <v>51</v>
+      </c>
+      <c r="N80" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="O80" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="L80" t="s">
-        <v>51</v>
-      </c>
-      <c r="M80" t="s">
-        <v>52</v>
-      </c>
-      <c r="N80" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="O80" s="5" t="s">
-        <v>66</v>
-      </c>
       <c r="V80" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="W80" t="s">
         <v>33</v>
@@ -4986,31 +4983,31 @@
         <v>366</v>
       </c>
       <c r="J81" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K81" t="s">
+        <v>335</v>
+      </c>
+      <c r="L81" t="s">
+        <v>50</v>
+      </c>
+      <c r="M81" t="s">
+        <v>37</v>
+      </c>
+      <c r="N81" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="O81" s="5" t="s">
         <v>336</v>
       </c>
-      <c r="L81" t="s">
-        <v>51</v>
-      </c>
-      <c r="M81" t="s">
-        <v>38</v>
-      </c>
-      <c r="N81" s="5" t="s">
+      <c r="V81" t="s">
+        <v>367</v>
+      </c>
+      <c r="W81" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z81" t="s">
         <v>338</v>
-      </c>
-      <c r="O81" s="5" t="s">
-        <v>337</v>
-      </c>
-      <c r="V81" t="s">
-        <v>368</v>
-      </c>
-      <c r="W81" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z81" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="82" spans="2:26" x14ac:dyDescent="0.2">
@@ -5027,28 +5024,28 @@
         <v>369</v>
       </c>
       <c r="J82" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K82" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="L82" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M82" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N82" s="5" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="O82" s="5" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="V82" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="W82" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="83" spans="2:26" x14ac:dyDescent="0.2">
@@ -5065,31 +5062,31 @@
         <v>372</v>
       </c>
       <c r="J83" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K83" t="s">
+        <v>342</v>
+      </c>
+      <c r="L83" t="s">
+        <v>50</v>
+      </c>
+      <c r="M83" t="s">
+        <v>37</v>
+      </c>
+      <c r="N83" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="O83" s="5" t="s">
         <v>343</v>
       </c>
-      <c r="L83" t="s">
-        <v>51</v>
-      </c>
-      <c r="M83" t="s">
-        <v>38</v>
-      </c>
-      <c r="N83" s="5" t="s">
+      <c r="V83" t="s">
+        <v>365</v>
+      </c>
+      <c r="W83" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z83" t="s">
         <v>345</v>
-      </c>
-      <c r="O83" s="5" t="s">
-        <v>344</v>
-      </c>
-      <c r="V83" t="s">
-        <v>366</v>
-      </c>
-      <c r="W83" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z83" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="84" spans="2:26" x14ac:dyDescent="0.2">
@@ -5106,31 +5103,31 @@
         <v>374</v>
       </c>
       <c r="J84" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K84" t="s">
+        <v>346</v>
+      </c>
+      <c r="L84" t="s">
+        <v>50</v>
+      </c>
+      <c r="M84" t="s">
+        <v>37</v>
+      </c>
+      <c r="N84" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="O84" s="5" t="s">
         <v>347</v>
       </c>
-      <c r="L84" t="s">
-        <v>51</v>
-      </c>
-      <c r="M84" t="s">
-        <v>38</v>
-      </c>
-      <c r="N84" s="5" t="s">
+      <c r="V84" t="s">
+        <v>368</v>
+      </c>
+      <c r="W84" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z84" t="s">
         <v>349</v>
-      </c>
-      <c r="O84" s="5" t="s">
-        <v>348</v>
-      </c>
-      <c r="V84" t="s">
-        <v>369</v>
-      </c>
-      <c r="W84" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z84" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="85" spans="2:26" x14ac:dyDescent="0.2">
@@ -5147,25 +5144,25 @@
         <v>388</v>
       </c>
       <c r="J85" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K85" t="s">
+        <v>163</v>
+      </c>
+      <c r="L85" t="s">
+        <v>50</v>
+      </c>
+      <c r="M85" t="s">
+        <v>37</v>
+      </c>
+      <c r="N85" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="O85" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="L85" t="s">
-        <v>51</v>
-      </c>
-      <c r="M85" t="s">
-        <v>38</v>
-      </c>
-      <c r="N85" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="O85" s="5" t="s">
-        <v>165</v>
-      </c>
       <c r="V85" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="W85" t="s">
         <v>33</v>
@@ -5185,31 +5182,31 @@
         <v>380</v>
       </c>
       <c r="J86" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K86" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="L86" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M86" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N86" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="O86" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="V86" t="s">
         <v>353</v>
       </c>
-      <c r="O86" s="5" t="s">
-        <v>352</v>
-      </c>
-      <c r="V86" t="s">
-        <v>354</v>
-      </c>
       <c r="W86" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Z86" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="87" spans="2:26" x14ac:dyDescent="0.2">
@@ -5226,31 +5223,31 @@
         <v>384</v>
       </c>
       <c r="J87" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K87" t="s">
+        <v>357</v>
+      </c>
+      <c r="L87" t="s">
+        <v>50</v>
+      </c>
+      <c r="M87" t="s">
+        <v>37</v>
+      </c>
+      <c r="N87" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="O87" s="5" t="s">
+        <v>354</v>
+      </c>
+      <c r="V87" t="s">
+        <v>364</v>
+      </c>
+      <c r="W87" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z87" t="s">
         <v>358</v>
-      </c>
-      <c r="L87" t="s">
-        <v>51</v>
-      </c>
-      <c r="M87" t="s">
-        <v>38</v>
-      </c>
-      <c r="N87" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="O87" s="5" t="s">
-        <v>355</v>
-      </c>
-      <c r="V87" t="s">
-        <v>365</v>
-      </c>
-      <c r="W87" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z87" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="88" spans="2:26" x14ac:dyDescent="0.2">
@@ -5267,31 +5264,31 @@
         <v>388</v>
       </c>
       <c r="J88" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K88" t="s">
+        <v>359</v>
+      </c>
+      <c r="L88" t="s">
+        <v>50</v>
+      </c>
+      <c r="M88" t="s">
+        <v>37</v>
+      </c>
+      <c r="N88" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="O88" s="5" t="s">
         <v>360</v>
       </c>
-      <c r="L88" t="s">
-        <v>51</v>
-      </c>
-      <c r="M88" t="s">
-        <v>38</v>
-      </c>
-      <c r="N88" s="5" t="s">
+      <c r="V88" t="s">
+        <v>363</v>
+      </c>
+      <c r="W88" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z88" t="s">
         <v>362</v>
-      </c>
-      <c r="O88" s="5" t="s">
-        <v>361</v>
-      </c>
-      <c r="V88" t="s">
-        <v>364</v>
-      </c>
-      <c r="W88" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z88" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="89" spans="2:26" x14ac:dyDescent="0.2">
@@ -5308,25 +5305,25 @@
         <v>399</v>
       </c>
       <c r="J89" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K89" t="s">
+        <v>376</v>
+      </c>
+      <c r="L89" t="s">
+        <v>50</v>
+      </c>
+      <c r="M89" t="s">
+        <v>51</v>
+      </c>
+      <c r="N89" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="O89" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="L89" t="s">
-        <v>51</v>
-      </c>
-      <c r="M89" t="s">
-        <v>52</v>
-      </c>
-      <c r="N89" s="5" t="s">
-        <v>379</v>
-      </c>
-      <c r="O89" s="5" t="s">
-        <v>378</v>
-      </c>
       <c r="V89" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="W89" t="s">
         <v>33</v>
@@ -5346,34 +5343,34 @@
         <v>391</v>
       </c>
       <c r="J90" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K90" t="s">
+        <v>371</v>
+      </c>
+      <c r="L90" t="s">
+        <v>50</v>
+      </c>
+      <c r="M90" t="s">
+        <v>41</v>
+      </c>
+      <c r="N90" s="5" t="s">
+        <v>373</v>
+      </c>
+      <c r="O90" s="5" t="s">
         <v>372</v>
       </c>
-      <c r="L90" t="s">
-        <v>51</v>
-      </c>
-      <c r="M90" t="s">
-        <v>42</v>
-      </c>
-      <c r="N90" s="5" t="s">
+      <c r="P90" s="5" t="s">
+        <v>375</v>
+      </c>
+      <c r="Q90" s="5" t="s">
         <v>374</v>
       </c>
-      <c r="O90" s="5" t="s">
-        <v>373</v>
-      </c>
-      <c r="P90" s="5" t="s">
-        <v>376</v>
-      </c>
-      <c r="Q90" s="5" t="s">
-        <v>375</v>
-      </c>
       <c r="V90" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="W90" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="91" spans="2:26" x14ac:dyDescent="0.2">
@@ -5390,28 +5387,28 @@
         <v>394</v>
       </c>
       <c r="J91" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K91" t="s">
+        <v>380</v>
+      </c>
+      <c r="L91" t="s">
+        <v>50</v>
+      </c>
+      <c r="M91" t="s">
+        <v>37</v>
+      </c>
+      <c r="N91" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="O91" s="5" t="s">
         <v>381</v>
       </c>
-      <c r="L91" t="s">
-        <v>51</v>
-      </c>
-      <c r="M91" t="s">
-        <v>38</v>
-      </c>
-      <c r="N91" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="O91" s="5" t="s">
-        <v>382</v>
-      </c>
       <c r="V91" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="W91" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="92" spans="2:26" x14ac:dyDescent="0.2">
@@ -5428,31 +5425,31 @@
         <v>396</v>
       </c>
       <c r="J92" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K92" t="s">
+        <v>384</v>
+      </c>
+      <c r="L92" t="s">
+        <v>50</v>
+      </c>
+      <c r="M92" t="s">
+        <v>41</v>
+      </c>
+      <c r="N92" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="O92" s="5" t="s">
         <v>385</v>
       </c>
-      <c r="L92" t="s">
-        <v>51</v>
-      </c>
-      <c r="M92" t="s">
-        <v>42</v>
-      </c>
-      <c r="N92" s="5" t="s">
+      <c r="V92" t="s">
+        <v>383</v>
+      </c>
+      <c r="W92" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z92" t="s">
         <v>387</v>
-      </c>
-      <c r="O92" s="5" t="s">
-        <v>386</v>
-      </c>
-      <c r="V92" t="s">
-        <v>384</v>
-      </c>
-      <c r="W92" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z92" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="93" spans="2:26" x14ac:dyDescent="0.2">
@@ -5469,28 +5466,28 @@
         <v>398</v>
       </c>
       <c r="J93" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K93" t="s">
+        <v>389</v>
+      </c>
+      <c r="L93" t="s">
+        <v>50</v>
+      </c>
+      <c r="M93" t="s">
+        <v>41</v>
+      </c>
+      <c r="N93" s="5" t="s">
+        <v>391</v>
+      </c>
+      <c r="O93" s="5" t="s">
         <v>390</v>
       </c>
-      <c r="L93" t="s">
-        <v>51</v>
-      </c>
-      <c r="M93" t="s">
-        <v>42</v>
-      </c>
-      <c r="N93" s="5" t="s">
-        <v>392</v>
-      </c>
-      <c r="O93" s="5" t="s">
-        <v>391</v>
-      </c>
       <c r="V93" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="W93" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="94" spans="2:26" x14ac:dyDescent="0.2">
@@ -5507,31 +5504,31 @@
         <v>399</v>
       </c>
       <c r="J94" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K94" t="s">
+        <v>392</v>
+      </c>
+      <c r="L94" t="s">
+        <v>50</v>
+      </c>
+      <c r="M94" t="s">
+        <v>41</v>
+      </c>
+      <c r="N94" s="5" t="s">
+        <v>395</v>
+      </c>
+      <c r="O94" s="5" t="s">
+        <v>394</v>
+      </c>
+      <c r="V94" t="s">
         <v>393</v>
       </c>
-      <c r="L94" t="s">
-        <v>51</v>
-      </c>
-      <c r="M94" t="s">
-        <v>42</v>
-      </c>
-      <c r="N94" s="5" t="s">
+      <c r="W94" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z94" t="s">
         <v>396</v>
-      </c>
-      <c r="O94" s="5" t="s">
-        <v>395</v>
-      </c>
-      <c r="V94" t="s">
-        <v>394</v>
-      </c>
-      <c r="W94" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z94" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="95" spans="2:26" x14ac:dyDescent="0.2">
@@ -5548,31 +5545,31 @@
         <v>401</v>
       </c>
       <c r="J95" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K95" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="L95" t="s">
+        <v>50</v>
+      </c>
+      <c r="M95" t="s">
         <v>51</v>
       </c>
-      <c r="M95" t="s">
-        <v>52</v>
-      </c>
       <c r="N95" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="O95" s="5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="V95" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="W95" t="s">
         <v>33</v>
       </c>
       <c r="Z95" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="96" spans="2:26" x14ac:dyDescent="0.2">
@@ -5589,31 +5586,31 @@
         <v>401</v>
       </c>
       <c r="J96" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K96" t="s">
+        <v>398</v>
+      </c>
+      <c r="L96" t="s">
+        <v>50</v>
+      </c>
+      <c r="M96" t="s">
+        <v>37</v>
+      </c>
+      <c r="N96" s="5" t="s">
+        <v>400</v>
+      </c>
+      <c r="O96" s="5" t="s">
         <v>399</v>
       </c>
-      <c r="L96" t="s">
-        <v>51</v>
-      </c>
-      <c r="M96" t="s">
-        <v>38</v>
-      </c>
-      <c r="N96" s="5" t="s">
-        <v>401</v>
-      </c>
-      <c r="O96" s="5" t="s">
-        <v>400</v>
-      </c>
       <c r="V96" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="W96" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Z96" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="97" spans="2:26" x14ac:dyDescent="0.2">
@@ -5630,31 +5627,31 @@
         <v>402</v>
       </c>
       <c r="J97" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K97" t="s">
+        <v>401</v>
+      </c>
+      <c r="L97" t="s">
+        <v>50</v>
+      </c>
+      <c r="M97" t="s">
+        <v>37</v>
+      </c>
+      <c r="N97" s="5" t="s">
+        <v>406</v>
+      </c>
+      <c r="O97" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="V97" t="s">
         <v>402</v>
-      </c>
-      <c r="L97" t="s">
-        <v>51</v>
-      </c>
-      <c r="M97" t="s">
-        <v>38</v>
-      </c>
-      <c r="N97" s="5" t="s">
-        <v>407</v>
-      </c>
-      <c r="O97" s="5" t="s">
-        <v>406</v>
-      </c>
-      <c r="V97" t="s">
-        <v>403</v>
       </c>
       <c r="W97" t="s">
         <v>33</v>
       </c>
       <c r="Z97" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="98" spans="2:26" x14ac:dyDescent="0.2">
@@ -5671,31 +5668,31 @@
         <v>402</v>
       </c>
       <c r="J98" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K98" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="L98" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M98" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N98" s="5" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="O98" s="5" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="V98" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="W98" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Z98" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="99" spans="2:26" x14ac:dyDescent="0.2">
@@ -5712,31 +5709,31 @@
         <v>404</v>
       </c>
       <c r="J99" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K99" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="L99" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M99" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N99" s="5" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="O99" s="5" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="V99" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="W99" t="s">
         <v>33</v>
       </c>
       <c r="Z99" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="100" spans="2:26" x14ac:dyDescent="0.2">
@@ -5753,31 +5750,31 @@
         <v>404</v>
       </c>
       <c r="J100" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K100" t="s">
+        <v>412</v>
+      </c>
+      <c r="L100" t="s">
+        <v>50</v>
+      </c>
+      <c r="M100" t="s">
+        <v>41</v>
+      </c>
+      <c r="N100" s="5" t="s">
+        <v>414</v>
+      </c>
+      <c r="O100" s="5" t="s">
         <v>413</v>
       </c>
-      <c r="L100" t="s">
-        <v>51</v>
-      </c>
-      <c r="M100" t="s">
-        <v>42</v>
-      </c>
-      <c r="N100" s="5" t="s">
+      <c r="V100" t="s">
+        <v>410</v>
+      </c>
+      <c r="W100" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z100" t="s">
         <v>415</v>
-      </c>
-      <c r="O100" s="5" t="s">
-        <v>414</v>
-      </c>
-      <c r="V100" t="s">
-        <v>411</v>
-      </c>
-      <c r="W100" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z100" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="101" spans="2:26" x14ac:dyDescent="0.2">
@@ -5794,25 +5791,25 @@
         <v>418</v>
       </c>
       <c r="J101" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K101" t="s">
+        <v>418</v>
+      </c>
+      <c r="L101" t="s">
+        <v>50</v>
+      </c>
+      <c r="M101" t="s">
+        <v>51</v>
+      </c>
+      <c r="N101" s="5" t="s">
+        <v>420</v>
+      </c>
+      <c r="O101" s="5" t="s">
         <v>419</v>
       </c>
-      <c r="L101" t="s">
-        <v>51</v>
-      </c>
-      <c r="M101" t="s">
-        <v>52</v>
-      </c>
-      <c r="N101" s="5" t="s">
-        <v>421</v>
-      </c>
-      <c r="O101" s="5" t="s">
-        <v>420</v>
-      </c>
       <c r="V101" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="W101" t="s">
         <v>31</v>
@@ -5832,25 +5829,25 @@
         <v>408</v>
       </c>
       <c r="J102" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K102" t="s">
+        <v>230</v>
+      </c>
+      <c r="L102" t="s">
+        <v>50</v>
+      </c>
+      <c r="M102" t="s">
+        <v>51</v>
+      </c>
+      <c r="N102" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="O102" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="L102" t="s">
-        <v>51</v>
-      </c>
-      <c r="M102" t="s">
-        <v>52</v>
-      </c>
-      <c r="N102" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="O102" s="5" t="s">
-        <v>232</v>
-      </c>
       <c r="V102" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="W102" t="s">
         <v>33</v>
@@ -5870,28 +5867,28 @@
         <v>408</v>
       </c>
       <c r="J103" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K103" t="s">
+        <v>421</v>
+      </c>
+      <c r="L103" t="s">
+        <v>50</v>
+      </c>
+      <c r="M103" t="s">
+        <v>37</v>
+      </c>
+      <c r="N103" s="5" t="s">
+        <v>423</v>
+      </c>
+      <c r="O103" s="5" t="s">
         <v>422</v>
       </c>
-      <c r="L103" t="s">
-        <v>51</v>
-      </c>
-      <c r="M103" t="s">
-        <v>38</v>
-      </c>
-      <c r="N103" s="5" t="s">
-        <v>424</v>
-      </c>
-      <c r="O103" s="5" t="s">
-        <v>423</v>
-      </c>
       <c r="V103" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="W103" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="104" spans="2:26" x14ac:dyDescent="0.2">
@@ -5908,25 +5905,25 @@
         <v>418</v>
       </c>
       <c r="J104" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K104" t="s">
+        <v>425</v>
+      </c>
+      <c r="L104" t="s">
+        <v>50</v>
+      </c>
+      <c r="M104" t="s">
+        <v>37</v>
+      </c>
+      <c r="N104" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="O104" s="5" t="s">
         <v>426</v>
       </c>
-      <c r="L104" t="s">
-        <v>51</v>
-      </c>
-      <c r="M104" t="s">
-        <v>38</v>
-      </c>
-      <c r="N104" s="5" t="s">
-        <v>428</v>
-      </c>
-      <c r="O104" s="5" t="s">
-        <v>427</v>
-      </c>
       <c r="V104" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="W104" t="s">
         <v>33</v>
@@ -5946,28 +5943,28 @@
         <v>409</v>
       </c>
       <c r="J105" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K105" t="s">
+        <v>428</v>
+      </c>
+      <c r="L105" t="s">
+        <v>50</v>
+      </c>
+      <c r="M105" t="s">
+        <v>37</v>
+      </c>
+      <c r="N105" s="5" t="s">
+        <v>430</v>
+      </c>
+      <c r="O105" s="5" t="s">
         <v>429</v>
       </c>
-      <c r="L105" t="s">
-        <v>51</v>
-      </c>
-      <c r="M105" t="s">
-        <v>38</v>
-      </c>
-      <c r="N105" s="5" t="s">
+      <c r="V105" t="s">
         <v>431</v>
       </c>
-      <c r="O105" s="5" t="s">
-        <v>430</v>
-      </c>
-      <c r="V105" t="s">
-        <v>432</v>
-      </c>
       <c r="W105" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="106" spans="2:26" x14ac:dyDescent="0.2">
@@ -5984,31 +5981,31 @@
         <v>411</v>
       </c>
       <c r="J106" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K106" t="s">
+        <v>433</v>
+      </c>
+      <c r="L106" t="s">
+        <v>50</v>
+      </c>
+      <c r="M106" t="s">
+        <v>37</v>
+      </c>
+      <c r="N106" s="5" t="s">
+        <v>435</v>
+      </c>
+      <c r="O106" s="5" t="s">
         <v>434</v>
       </c>
-      <c r="L106" t="s">
-        <v>51</v>
-      </c>
-      <c r="M106" t="s">
-        <v>38</v>
-      </c>
-      <c r="N106" s="5" t="s">
+      <c r="V106" t="s">
+        <v>432</v>
+      </c>
+      <c r="W106" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z106" t="s">
         <v>436</v>
-      </c>
-      <c r="O106" s="5" t="s">
-        <v>435</v>
-      </c>
-      <c r="V106" t="s">
-        <v>433</v>
-      </c>
-      <c r="W106" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z106" t="s">
-        <v>437</v>
       </c>
     </row>
     <row r="107" spans="2:26" x14ac:dyDescent="0.2">
@@ -6025,28 +6022,28 @@
         <v>412</v>
       </c>
       <c r="J107" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K107" t="s">
+        <v>438</v>
+      </c>
+      <c r="L107" t="s">
+        <v>50</v>
+      </c>
+      <c r="M107" t="s">
+        <v>37</v>
+      </c>
+      <c r="N107" s="5" t="s">
+        <v>440</v>
+      </c>
+      <c r="O107" s="5" t="s">
         <v>439</v>
       </c>
-      <c r="L107" t="s">
-        <v>51</v>
-      </c>
-      <c r="M107" t="s">
-        <v>38</v>
-      </c>
-      <c r="N107" s="5" t="s">
-        <v>441</v>
-      </c>
-      <c r="O107" s="5" t="s">
-        <v>440</v>
-      </c>
       <c r="V107" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="W107" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="108" spans="2:26" x14ac:dyDescent="0.2">
@@ -6063,28 +6060,28 @@
         <v>413</v>
       </c>
       <c r="J108" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K108" t="s">
+        <v>442</v>
+      </c>
+      <c r="L108" t="s">
+        <v>50</v>
+      </c>
+      <c r="M108" t="s">
+        <v>37</v>
+      </c>
+      <c r="N108" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="O108" s="5" t="s">
         <v>443</v>
       </c>
-      <c r="L108" t="s">
-        <v>51</v>
-      </c>
-      <c r="M108" t="s">
-        <v>38</v>
-      </c>
-      <c r="N108" s="5" t="s">
-        <v>445</v>
-      </c>
-      <c r="O108" s="5" t="s">
-        <v>444</v>
-      </c>
       <c r="V108" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="W108" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="109" spans="2:26" x14ac:dyDescent="0.2">
@@ -6101,31 +6098,31 @@
         <v>415</v>
       </c>
       <c r="J109" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K109" t="s">
+        <v>446</v>
+      </c>
+      <c r="L109" t="s">
+        <v>50</v>
+      </c>
+      <c r="M109" t="s">
+        <v>37</v>
+      </c>
+      <c r="N109" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="O109" s="5" t="s">
         <v>447</v>
       </c>
-      <c r="L109" t="s">
-        <v>51</v>
-      </c>
-      <c r="M109" t="s">
-        <v>38</v>
-      </c>
-      <c r="N109" s="5" t="s">
+      <c r="V109" t="s">
+        <v>445</v>
+      </c>
+      <c r="W109" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z109" t="s">
         <v>449</v>
-      </c>
-      <c r="O109" s="5" t="s">
-        <v>448</v>
-      </c>
-      <c r="V109" t="s">
-        <v>446</v>
-      </c>
-      <c r="W109" t="s">
-        <v>82</v>
-      </c>
-      <c r="Z109" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="110" spans="2:26" x14ac:dyDescent="0.2">
@@ -6142,28 +6139,28 @@
         <v>416</v>
       </c>
       <c r="J110" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K110" t="s">
+        <v>451</v>
+      </c>
+      <c r="L110" t="s">
+        <v>50</v>
+      </c>
+      <c r="M110" t="s">
+        <v>37</v>
+      </c>
+      <c r="N110" s="5" t="s">
+        <v>453</v>
+      </c>
+      <c r="O110" s="5" t="s">
         <v>452</v>
       </c>
-      <c r="L110" t="s">
-        <v>51</v>
-      </c>
-      <c r="M110" t="s">
-        <v>38</v>
-      </c>
-      <c r="N110" s="5" t="s">
-        <v>454</v>
-      </c>
-      <c r="O110" s="5" t="s">
-        <v>453</v>
-      </c>
       <c r="V110" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="W110" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="111" spans="2:26" x14ac:dyDescent="0.2">
@@ -6180,28 +6177,28 @@
         <v>418</v>
       </c>
       <c r="J111" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K111" t="s">
+        <v>455</v>
+      </c>
+      <c r="L111" t="s">
+        <v>50</v>
+      </c>
+      <c r="M111" t="s">
+        <v>37</v>
+      </c>
+      <c r="N111" s="5" t="s">
+        <v>457</v>
+      </c>
+      <c r="O111" s="5" t="s">
         <v>456</v>
       </c>
-      <c r="L111" t="s">
-        <v>51</v>
-      </c>
-      <c r="M111" t="s">
-        <v>38</v>
-      </c>
-      <c r="N111" s="5" t="s">
-        <v>458</v>
-      </c>
-      <c r="O111" s="5" t="s">
-        <v>457</v>
-      </c>
       <c r="V111" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="W111" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>